<commit_message>
Smoke test script now works
</commit_message>
<xml_diff>
--- a/issue_template.xlsx
+++ b/issue_template.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Title</t>
   </si>
@@ -149,41 +149,7 @@
 - [ ] Run through some examples from [the documentation](http://www.mantidproject.org/Python_In_Mantid), 3 or 4 examples is enough </t>
   </si>
   <si>
-    <t>Smoke Testing Umbrella Issue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is to keep track of the coverage of smoke tests during the release cycle.
-Edit this Issue and Mark beside your OS on the Test you are going to complete.
-eg. Windows  - @DanielMurphy22
-## Clean/Dirty Install Smoke Tests: 
- - [ ] Windows 
- - [ ] OSX  
- - [ ] Linux
-## Fitting Smoke Tests: 
- - [ ] Windows 
- - [ ] OSX 
- - [ ] Linux
- - [ ] IDaaS  
-## Interface Smoke Tests: 
- - [ ] Windows  
- - [ ] OSX 
- - [ ] Linux
- - [ ] IDaaS 
-## Plotting Smoke Tests: 
- - [ ] Windows  
- - [ ] OSX 
- - [ ] Linux 
- - [ ] IDaaS  
-## Python Smoke Tests: 
- - [ ] Windows  
- - [ ] OSX  
- - [ ] Linux  
- - [ ] IDaaS  
-## Workspace/Algorithm Smoke Tests:
- - [ ] Windows 
- - [ ] OSX 
- - [ ] Linux  
- - [ ] IDaaS </t>
+    <t>DanielMurphy22</t>
   </si>
 </sst>
 </file>
@@ -191,7 +157,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -694,7 +660,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1062,7 +1028,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,7 +1057,9 @@
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2"/>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1127,7 +1095,9 @@
       <c r="B6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6"/>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1138,13 +1108,8 @@
       </c>
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>16</v>
-      </c>
+    <row r="8" spans="1:3" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="C8"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,26 +1188,23 @@
       <c r="C33"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F7"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C33">
+      <formula1>#REF!</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>[issue_templateupdate.xlsx]assignees!#REF!</xm:f>
           </x14:formula1>
           <xm:sqref>C34:C40</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>C2:C33</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>

</xml_diff>